<commit_message>
Sum expenses + save cost as float :bear:
</commit_message>
<xml_diff>
--- a/python/openpyxl/expenses.xlsx
+++ b/python/openpyxl/expenses.xlsx
@@ -16,24 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+  <si>
+    <t>Cha Yen</t>
+  </si>
   <si>
     <t>Beef Steak</t>
-  </si>
-  <si>
-    <t>350</t>
-  </si>
-  <si>
-    <t>Candy</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Kra Pow Kai</t>
-  </si>
-  <si>
-    <t>55</t>
   </si>
 </sst>
 </file>
@@ -390,7 +378,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -398,37 +386,30 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="n">
         <v>43496</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
+      <c r="C1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D1">
+        <f>SUM(C1:C2)</f>
+        <v/>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="n">
         <v>43496</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="n">
-        <v>43496</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>